<commit_message>
Adding Authentication and Authorization;
</commit_message>
<xml_diff>
--- a/MERN.xlsx
+++ b/MERN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\202302_MERN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D066F6E7-CB22-4644-9BC5-9C9E1782F660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C91793-6242-4323-AF50-E58149565262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40890" yWindow="3630" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21270" yWindow="780" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="654">
   <si>
     <t>https://www.udemy.com/course/react-nodejs-express-mongodb-the-mern-fullstack-guide/</t>
   </si>
@@ -2947,6 +2947,326 @@
   </si>
   <si>
     <t>How Authentication works?</t>
+  </si>
+  <si>
+    <t>So sánh giữa Cookie và Token.</t>
+  </si>
+  <si>
+    <t>Ví dụ: load balancing giữa server A và server B</t>
+  </si>
+  <si>
+    <t>+ Token = Stateless -&gt; scalability</t>
+  </si>
+  <si>
+    <t>+ Hỗ trợ mobile</t>
+  </si>
+  <si>
+    <t>+ Hỗ trợ Multi-Server Platforms And Distributed Micro-Services</t>
+  </si>
+  <si>
+    <t>Sử dụng thư biện bcryptjs</t>
+  </si>
+  <si>
+    <t>$ npm install --save bcryptjs</t>
+  </si>
+  <si>
+    <t>Hash password (signup)</t>
+  </si>
+  <si>
+    <t>Compare password (login)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hashedPassword = await </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bcrypt.hash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(password, 12);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">isValid = await </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bcrypt.compare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(password, existingUser.password);</t>
+    </r>
+  </si>
+  <si>
+    <t>Encrypt password</t>
+  </si>
+  <si>
+    <t>Generate token (JWT)</t>
+  </si>
+  <si>
+    <t>Storing the token in the Browser Storage</t>
+  </si>
+  <si>
+    <t>Sử dụng thư viện jsonwebtoken</t>
+  </si>
+  <si>
+    <t>$ npm install --save jsonwebtoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinh token </t>
+  </si>
+  <si>
+    <t>let token;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    { userId: existingUser.id, email: existingUser.email },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    process.env.JWT_KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    { expiresIn: '1h' }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  return next(new HttpError('Login failed. Please try again.', 500));</t>
+  </si>
+  <si>
+    <t>Trả về token</t>
+  </si>
+  <si>
+    <t>res.status(200).json({</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  userId: existingUser.id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  email: existingUser.email,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  token: token,</t>
+  </si>
+  <si>
+    <t>// trong token chứa userId và email</t>
+  </si>
+  <si>
+    <t>Authentication middleware</t>
+  </si>
+  <si>
+    <t>// by pass OPTIONS request</t>
+  </si>
+  <si>
+    <t>if (req.method === 'OPTIONS') {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  return next();</t>
+  </si>
+  <si>
+    <t>// Authorization: 'Bearer TOKEN'</t>
+  </si>
+  <si>
+    <t>const token = req.headers.authorization.split(' ')[1];</t>
+  </si>
+  <si>
+    <t>console.log(`decodedToken: ${JSON.stringify(decodedToken)}`);</t>
+  </si>
+  <si>
+    <t>req.userData = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  userId: decodedToken.userId,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  email: decodedToken.email</t>
+  </si>
+  <si>
+    <t>next();</t>
+  </si>
+  <si>
+    <t>// bỏ qua OPTIONS request từ Browser</t>
+  </si>
+  <si>
+    <t>// Token sẽ có dạng Bearer …</t>
+  </si>
+  <si>
+    <t>// Đính kèm userData vào request để phục vụ các xử lý tiếp theo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const decodedToken = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jwt.verify(token, process.env.JWT_KEY);</t>
+    </r>
+  </si>
+  <si>
+    <t>// Tách lấy token</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  token = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jwt.sign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <t>NOTE: Kiểm tra thông tin user khi thực hiện UPDATE/DELETE - phải đúng là user creator</t>
+  </si>
+  <si>
+    <t>// Only creator can delete the place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  const error = new HttpError('You are not allowed to delete this place.', 401);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  return next(error);</t>
+  </si>
+  <si>
+    <r>
+      <t>if (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>req.userData.userId !== place.creator.id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <t>Bảo vệ Route bằng authentication middleware: ví dụ place-routes.js</t>
+  </si>
+  <si>
+    <r>
+      <t>router.use(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkAuth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>const checkAuth = require('../middleware/check-auth');</t>
+  </si>
+  <si>
+    <t>Browser cung cấp một số storage</t>
+  </si>
+  <si>
+    <t>IndexedDB</t>
+  </si>
+  <si>
+    <t>Session Storage</t>
+  </si>
+  <si>
+    <t>Local Storage</t>
+  </si>
+  <si>
+    <t>Bị xóa mỗi khi đóng browser</t>
+  </si>
+  <si>
+    <t>Persist khi restart browser và cache</t>
+  </si>
+  <si>
+    <t>Phức tạp</t>
+  </si>
+  <si>
+    <t>Lưu token vào local storage</t>
+  </si>
+  <si>
+    <t>Quản lý Token expiration date</t>
+  </si>
+  <si>
+    <t>Auto log-out khi token expired</t>
+  </si>
+  <si>
+    <t>Auto log-in khi refresh</t>
   </si>
 </sst>
 </file>
@@ -3099,7 +3419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3123,6 +3443,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3968,6 +4289,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>596442</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B3B9852-F9C2-43E3-A60C-C4EAC18970F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="1535206"/>
+          <a:ext cx="6647619" cy="3009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4422,6 +4792,9 @@
       <c r="I17" s="5" t="s">
         <v>587</v>
       </c>
+      <c r="J17" s="7">
+        <v>45016</v>
+      </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -4476,7 +4849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3139FA3-25F2-4153-A6D2-67965DFF0247}">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -7409,9 +7782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B935B4-87C8-4392-B24C-8C5B7B922FCD}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7619,30 +7990,395 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EECA97-437D-4195-8BA5-2492DDFD6A0A}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="8" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="8" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="13" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="13" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="13" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D33" s="13" t="s">
+        <v>608</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="13" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D35" s="13" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D36" s="13" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D37" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D38" s="13" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D41" s="13" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="13" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="13" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="21" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D47" s="13" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D48" s="13" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D50" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D51" s="13" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="13" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D55" s="13" t="s">
+        <v>622</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="13" t="s">
+        <v>623</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D57" s="13" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D58" s="13" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D59" s="13" t="s">
+        <v>625</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D60" s="13" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D61" s="13" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D62" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D63" s="13" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C64" s="18" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D65" s="13" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D66" s="13" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D67" s="13" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D68" s="13" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D69" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D73" s="23" t="s">
+        <v>644</v>
+      </c>
+      <c r="F73" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D74" s="23" t="s">
+        <v>645</v>
+      </c>
+      <c r="F74" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D75" s="23" t="s">
+        <v>646</v>
+      </c>
+      <c r="F75" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -7650,5 +8386,7 @@
     <hyperlink ref="A1" location="Intro!A1" display="Intro" xr:uid="{2528F162-F0F3-4DB4-BA4F-5594727E31DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>